<commit_message>
Criação de metodo para salvar resultado d teste na planilha
Metodo pushData salva o resultado do teste na planilha
</commit_message>
<xml_diff>
--- a/testes/teste-de-software-automatizado/data/cases.xlsx
+++ b/testes/teste-de-software-automatizado/data/cases.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr checkCompatibility="1" defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Projeto Ailton\admintcc\admintcc\testes\teste-de-software-automatizado\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15885" windowHeight="6525" firstSheet="2" activeTab="4"/>
   </bookViews>
@@ -14,12 +19,11 @@
     <sheet name="Login" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <oleSize ref="A1:P23"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="15">
   <si>
     <t>TestCase</t>
   </si>
@@ -61,6 +65,9 @@
   </si>
   <si>
     <t>senha123</t>
+  </si>
+  <si>
+    <t>Conclído</t>
   </si>
 </sst>
 </file>
@@ -435,7 +442,9 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="G2" s="3" t="s">
         <v>8</v>
@@ -629,10 +638,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -676,7 +685,11 @@
         <v>13</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D3" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Complementações no script de testes
Criação do metodo toCompared
</commit_message>
<xml_diff>
--- a/testes/teste-de-software-automatizado/data/cases.xlsx
+++ b/testes/teste-de-software-automatizado/data/cases.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr checkCompatibility="1" defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Projeto Ailton\admintcc\admintcc\testes\teste-de-software-automatizado\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15885" windowHeight="6525" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21075" windowHeight="10695"/>
   </bookViews>
   <sheets>
     <sheet name="CadastroAluno" sheetId="1" r:id="rId1"/>
@@ -18,12 +13,13 @@
     <sheet name="CadastroSupervisor" sheetId="4" r:id="rId4"/>
     <sheet name="Login" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:H10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="16">
   <si>
     <t>TestCase</t>
   </si>
@@ -67,14 +63,18 @@
     <t>senha123</t>
   </si>
   <si>
-    <t>Conclído</t>
+    <t>Cadastrar Projeto TCC</t>
+  </si>
+  <si>
+    <t>passed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -95,6 +95,20 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -118,11 +132,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -406,11 +422,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="A1:H2"/>
+    <sheetView tabSelected="1" zoomScale="250" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -422,18 +442,13 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -442,26 +457,24 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="E2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D3" s="1"/>
+      <c r="D3" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -470,7 +483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="250" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -526,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H2"/>
+    <sheetView topLeftCell="A2" zoomScale="250" workbookViewId="0">
+      <selection activeCell="C11" sqref="C10:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -583,7 +596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="250" workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -640,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Criação dos metodos para salvar as evidências
Método que cria imagens a cada movimento do teste
</commit_message>
<xml_diff>
--- a/testes/teste-de-software-automatizado/data/cases.xlsx
+++ b/testes/teste-de-software-automatizado/data/cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr checkCompatibility="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21075" windowHeight="10695"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21075" windowHeight="7575"/>
   </bookViews>
   <sheets>
     <sheet name="CadastroAluno" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="16">
   <si>
     <t>TestCase</t>
   </si>
@@ -73,7 +73,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -423,13 +422,13 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="250" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Complementações script de testes
</commit_message>
<xml_diff>
--- a/testes/teste-de-software-automatizado/data/cases.xlsx
+++ b/testes/teste-de-software-automatizado/data/cases.xlsx
@@ -14,12 +14,12 @@
     <sheet name="Login" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H10"/>
+  <oleSize ref="D1:J10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="26">
   <si>
     <t>TestCase</t>
   </si>
@@ -63,7 +63,37 @@
     <t>senha123</t>
   </si>
   <si>
-    <t>Cadastrar Projeto TCC</t>
+    <t>link</t>
+  </si>
+  <si>
+    <t>http://ronivonmendes.tk/iftm/admintcc/login.php</t>
+  </si>
+  <si>
+    <t>nome</t>
+  </si>
+  <si>
+    <t>Aluno Teste</t>
+  </si>
+  <si>
+    <t>rg</t>
+  </si>
+  <si>
+    <t>Mg-17.568.166</t>
+  </si>
+  <si>
+    <t>oi</t>
+  </si>
+  <si>
+    <t>orgao</t>
+  </si>
+  <si>
+    <t>PF</t>
+  </si>
+  <si>
+    <t>cpf</t>
+  </si>
+  <si>
+    <t>12684613600</t>
   </si>
   <si>
     <t>passed</t>
@@ -73,6 +103,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -131,13 +162,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -419,19 +452,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="250" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,9 +480,20 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -457,18 +501,38 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D3" s="2"/>
     </row>
   </sheetData>
@@ -650,7 +714,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
@@ -658,7 +722,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -680,8 +744,11 @@
       <c r="H1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -696,8 +763,11 @@
       <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D3" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alterações em testes e no BD
</commit_message>
<xml_diff>
--- a/testes/teste-de-software-automatizado/data/cases.xlsx
+++ b/testes/teste-de-software-automatizado/data/cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr checkCompatibility="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21075" windowHeight="7575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="3360" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CadastroAluno" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <sheet name="Login" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="D1:J10"/>
+  <oleSize ref="G1:O2"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="52">
   <si>
     <t>TestCase</t>
   </si>
@@ -72,18 +72,12 @@
     <t>nome</t>
   </si>
   <si>
-    <t>Aluno Teste</t>
-  </si>
-  <si>
     <t>rg</t>
   </si>
   <si>
     <t>Mg-17.568.166</t>
   </si>
   <si>
-    <t>oi</t>
-  </si>
-  <si>
     <t>orgao</t>
   </si>
   <si>
@@ -96,21 +90,119 @@
     <t>12684613600</t>
   </si>
   <si>
+    <t>curso</t>
+  </si>
+  <si>
+    <t>Processos Químicos - (Graduação)</t>
+  </si>
+  <si>
+    <t>matricula</t>
+  </si>
+  <si>
+    <t>telefone</t>
+  </si>
+  <si>
+    <t>99998888</t>
+  </si>
+  <si>
+    <t>cep</t>
+  </si>
+  <si>
+    <t>38304258</t>
+  </si>
+  <si>
+    <t>numero</t>
+  </si>
+  <si>
+    <t>2213</t>
+  </si>
+  <si>
+    <t>Aluno teste</t>
+  </si>
+  <si>
+    <t>senhateste</t>
+  </si>
+  <si>
+    <t>Aluno cadastrado com sucesso!</t>
+  </si>
+  <si>
+    <t>alunoteste3@mail.com</t>
+  </si>
+  <si>
+    <t>passed</t>
+  </si>
+  <si>
+    <t>CadastroOrientaor</t>
+  </si>
+  <si>
+    <t>titulacao</t>
+  </si>
+  <si>
+    <t>instituicao</t>
+  </si>
+  <si>
+    <t>orientador teste</t>
+  </si>
+  <si>
+    <t>MG-14.123.123</t>
+  </si>
+  <si>
+    <t>12345678910</t>
+  </si>
+  <si>
+    <t>Mestre</t>
+  </si>
+  <si>
+    <r>
+      <t>IFTM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF545454"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF6A6A6A"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Instituto Federal do Triângulo Mineiro</t>
+    </r>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>orientador@mail.com</t>
+  </si>
+  <si>
+    <t>corientador teste</t>
+  </si>
+  <si>
+    <t>coorientador@mail.com</t>
+  </si>
+  <si>
+    <t>Cadastro realizado com sucesso!</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>papagaio</t>
-  </si>
-  <si>
-    <t>passed</t>
+    <t>CadastroCoorientador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -146,6 +238,19 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF6A6A6A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF545454"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -168,7 +273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -177,6 +282,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -460,14 +567,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
@@ -490,13 +597,34 @@
         <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -507,33 +635,47 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
+      <c r="M2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="Q2" s="7"/>
       <c r="R2" s="7"/>
       <c r="S2" s="7"/>
@@ -542,23 +684,26 @@
       <c r="D3" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView zoomScale="250" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -574,30 +719,90 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="P1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="O2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
@@ -606,15 +811,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="250" workbookViewId="0">
-      <selection activeCell="C11" sqref="C10:C11"/>
+    <sheetView zoomScale="160" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -630,34 +835,108 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="P1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="1"/>
       <c r="D2" s="2"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="O2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -722,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView zoomScale="115" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -769,7 +1048,7 @@
       <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -777,7 +1056,10 @@
       <c r="D3" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Alteração na base de testes
</commit_message>
<xml_diff>
--- a/testes/teste-de-software-automatizado/data/cases.xlsx
+++ b/testes/teste-de-software-automatizado/data/cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr checkCompatibility="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21075" windowHeight="7575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10995" windowHeight="3135"/>
   </bookViews>
   <sheets>
     <sheet name="CadastroAluno" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,12 @@
     <sheet name="Login" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:Q23"/>
+  <oleSize ref="E1:M8"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="74">
   <si>
     <t>TestCase</t>
   </si>
@@ -175,88 +175,101 @@
     <t>CadastroCoorientador</t>
   </si>
   <si>
+    <t>CT01</t>
+  </si>
+  <si>
+    <t>bep</t>
+  </si>
+  <si>
+    <t>CadastroSupervisor</t>
+  </si>
+  <si>
+    <t>Projeto cadastrado com sucesso!</t>
+  </si>
+  <si>
+    <t>emailOrientador</t>
+  </si>
+  <si>
+    <t>senhaOrientador</t>
+  </si>
+  <si>
+    <t>nomeAluno</t>
+  </si>
+  <si>
+    <t>titulo</t>
+  </si>
+  <si>
+    <t>ProjetoTCCBB</t>
+  </si>
+  <si>
+    <t>grupo</t>
+  </si>
+  <si>
+    <t>Química aplicada</t>
+  </si>
+  <si>
+    <t>mensagem</t>
+  </si>
+  <si>
+    <t>emailAluno</t>
+  </si>
+  <si>
+    <t>senhaAluno</t>
+  </si>
+  <si>
+    <t>resumo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O resumo de um tecc </t>
+  </si>
+  <si>
+    <t>coorientador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador Master (Instituto Federal de Educação, Ciência e Tecnologia do Triângulo Mineiro) </t>
+  </si>
+  <si>
+    <t>orientadorGH@mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>orientador GH</t>
+  </si>
+  <si>
+    <t>supervisor1111@mail.com</t>
+  </si>
+  <si>
+    <t>Supervisor testes 1111</t>
+  </si>
+  <si>
+    <t>coorientador88822@mail.com</t>
+  </si>
+  <si>
+    <t>Aluno AA</t>
+  </si>
+  <si>
+    <t>alunoAA@mail.com</t>
+  </si>
+  <si>
+    <t>Adelino Pessanha</t>
+  </si>
+  <si>
+    <t>adelinopessanha@gmail.com</t>
+  </si>
+  <si>
+    <t>239048209348203</t>
+  </si>
+  <si>
     <t>passed</t>
-  </si>
-  <si>
-    <t>CT01</t>
-  </si>
-  <si>
-    <t>bep</t>
-  </si>
-  <si>
-    <t>Supervisor testes</t>
-  </si>
-  <si>
-    <t>supervisor@mail.com</t>
-  </si>
-  <si>
-    <t>CadastroSupervisor</t>
-  </si>
-  <si>
-    <t>coorientador2222@mail.com</t>
-  </si>
-  <si>
-    <t>orientador14@mail.com</t>
-  </si>
-  <si>
-    <t>orientador teste14</t>
-  </si>
-  <si>
-    <t>Aluno teste14</t>
-  </si>
-  <si>
-    <t>alunoteste14@mail.com</t>
-  </si>
-  <si>
-    <t>Projeto cadastrado com sucesso!</t>
-  </si>
-  <si>
-    <t>emailOrientador</t>
-  </si>
-  <si>
-    <t>senhaOrientador</t>
-  </si>
-  <si>
-    <t>nomeAluno</t>
-  </si>
-  <si>
-    <t>aluno teste14</t>
-  </si>
-  <si>
-    <t>titulo</t>
-  </si>
-  <si>
-    <t>ProjetoTCCBB</t>
-  </si>
-  <si>
-    <t>grupo</t>
-  </si>
-  <si>
-    <t>Química aplicada</t>
-  </si>
-  <si>
-    <t>mensagem</t>
-  </si>
-  <si>
-    <t>emailAluno</t>
-  </si>
-  <si>
-    <t>aluno14@mail.com</t>
-  </si>
-  <si>
-    <t>senhaAluno</t>
-  </si>
-  <si>
-    <t>resumo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O resumo de um tecc </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -328,7 +341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -339,6 +352,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -620,16 +634,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
@@ -681,9 +695,6 @@
       <c r="P1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -693,7 +704,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>31</v>
@@ -702,7 +713,7 @@
         <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>16</v>
@@ -717,7 +728,7 @@
         <v>22</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>25</v>
@@ -729,20 +740,23 @@
         <v>29</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="6" t="s">
-        <v>69</v>
-      </c>
       <c r="R2" s="7"/>
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D3" s="2"/>
+      <c r="M3" s="1"/>
       <c r="Q3" s="2"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="O14" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -756,15 +770,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView topLeftCell="D1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -781,69 +795,79 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H1" t="s">
+      <c r="N1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I1" t="s">
+      <c r="O1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="C2" s="4"/>
       <c r="D2" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" t="s">
-        <v>30</v>
+        <v>62</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="I2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="J2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>30</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -852,13 +876,13 @@
     <hyperlink ref="L2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
@@ -866,7 +890,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -904,7 +928,7 @@
         <v>24</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>28</v>
@@ -916,7 +940,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -924,7 +948,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
         <v>41</v>
@@ -957,7 +981,7 @@
         <v>29</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>11</v>
@@ -974,15 +998,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="F1" zoomScale="115" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1032,7 +1056,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -1045,7 +1069,7 @@
         <v>41</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>35</v>
@@ -1072,12 +1096,12 @@
         <v>29</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="6"/>
+      <c r="Q2" s="10"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
@@ -1105,15 +1129,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView zoomScale="115" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1163,9 +1187,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1175,7 +1199,7 @@
         <v>41</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>35</v>
@@ -1202,7 +1226,7 @@
         <v>29</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>11</v>

</xml_diff>